<commit_message>
Improvements: - Improved: Auto add file suffix after incorrect manual edit of file path Bugfix: - Fixed: Typo in default Specific_ions config file
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/3-Specific_ions.xlsx
+++ b/ConfigurationFiles/3-Specific_ions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0E803216-F459-439F-9484-18BC6E6C3605}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BC8D9EED-6E73-4597-8131-5F4CF1F705D2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -271,15 +271,6 @@
     <t>PE Head Group in positive mode</t>
   </si>
   <si>
-    <t>C2H9O4NP-</t>
-  </si>
-  <si>
-    <t>C5H15NO4P-</t>
-  </si>
-  <si>
-    <t>C3H9NO6P-</t>
-  </si>
-  <si>
     <t>PS:186</t>
   </si>
   <si>
@@ -289,9 +280,6 @@
     <t>TG ammonium loss</t>
   </si>
   <si>
-    <t>NH3+H2O</t>
-  </si>
-  <si>
     <t>TG ammonium loss + water</t>
   </si>
   <si>
@@ -305,6 +293,18 @@
   </si>
   <si>
     <t>DG</t>
+  </si>
+  <si>
+    <t>C3H9NO6P+</t>
+  </si>
+  <si>
+    <t>C5H15NO4P+</t>
+  </si>
+  <si>
+    <t>C2H9O4NP+</t>
+  </si>
+  <si>
+    <t>NH5O</t>
   </si>
 </sst>
 </file>
@@ -676,7 +676,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G1:G1048576"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1011,7 +1011,7 @@
         <v>184.07390000000001</v>
       </c>
       <c r="D14" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>75</v>
@@ -1150,7 +1150,7 @@
         <v>142.02690000000001</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="E20" s="5" t="s">
         <v>75</v>
@@ -1358,7 +1358,7 @@
         <v>186.01679999999999</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>75</v>
@@ -1367,10 +1367,10 @@
         <v>74</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1400,12 +1400,12 @@
         <v>74</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>4</v>
@@ -1414,7 +1414,7 @@
         <v>35.037114000000003</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>75</v>
@@ -1423,15 +1423,15 @@
         <v>80</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>4</v>
@@ -1440,7 +1440,7 @@
         <v>18.010565</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E35" s="5" t="s">
         <v>75</v>
@@ -1449,10 +1449,10 @@
         <v>74</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prepare for LipidHunter 2 release
NewFeatures:
+ New: Change RT,m/z range based on user selections
+ New: User guide in PDF
+ New: python requirements list
+ New: KNIME sample workflow

Changes:
+ Changed: Merge FA list into one
+ Changed: UI updated
+ Changed: Update Readme file

BugFix:
+ Fixed: Typo in Specific_ions
</commit_message>
<xml_diff>
--- a/ConfigurationFiles/3-Specific_ions.xlsx
+++ b/ConfigurationFiles/3-Specific_ions.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BC8D9EED-6E73-4597-8131-5F4CF1F705D2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -202,15 +201,6 @@
     <t>PE Head Group [M-H]-</t>
   </si>
   <si>
-    <t>Deprotonated doubly dehydrated glycerol phosphocholine</t>
-  </si>
-  <si>
-    <t>-PE Head Group</t>
-  </si>
-  <si>
-    <t>-PE Head Group part</t>
-  </si>
-  <si>
     <t>PG Head Group [M-H]-</t>
   </si>
   <si>
@@ -259,9 +249,6 @@
     <t>PC:184</t>
   </si>
   <si>
-    <t>PC Head Group ion in positive mode</t>
-  </si>
-  <si>
     <t>[M+NH4]+</t>
   </si>
   <si>
@@ -305,12 +292,24 @@
   </si>
   <si>
     <t>NH5O</t>
+  </si>
+  <si>
+    <t>Deprotonated dehydrated glycerol phosphoethanolamine [M-H]-</t>
+  </si>
+  <si>
+    <t>-PE Head Group [M-H]-</t>
+  </si>
+  <si>
+    <t>-PE Head Group part [M-H]-</t>
+  </si>
+  <si>
+    <t>PC Head Group ion in positive mode [M+H]+</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -672,23 +671,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="11.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="7" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11.7265625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.54296875" customWidth="1"/>
+    <col min="5" max="5" width="15.26953125" customWidth="1"/>
+    <col min="6" max="7" width="13.54296875" customWidth="1"/>
     <col min="8" max="8" width="68" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -714,7 +713,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>40</v>
       </c>
@@ -740,7 +739,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -766,7 +765,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -792,7 +791,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -818,7 +817,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>0</v>
       </c>
@@ -844,7 +843,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
@@ -870,7 +869,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
@@ -887,7 +886,7 @@
         <v>48</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>28</v>
@@ -896,7 +895,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>0</v>
       </c>
@@ -913,7 +912,7 @@
         <v>48</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>29</v>
@@ -922,7 +921,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>0</v>
       </c>
@@ -939,7 +938,7 @@
         <v>48</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>30</v>
@@ -948,7 +947,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>0</v>
       </c>
@@ -959,22 +958,22 @@
         <v>74.036779999999993</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>48</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>0</v>
       </c>
@@ -991,7 +990,7 @@
         <v>48</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>52</v>
@@ -1000,7 +999,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
@@ -1011,22 +1010,22 @@
         <v>184.07390000000001</v>
       </c>
       <c r="D14" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E14" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>78</v>
-      </c>
       <c r="H14" s="4" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="3"/>
@@ -1035,7 +1034,7 @@
       <c r="G15" s="5"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>11</v>
       </c>
@@ -1061,7 +1060,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>11</v>
       </c>
@@ -1084,10 +1083,10 @@
         <v>33</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>11</v>
       </c>
@@ -1110,10 +1109,10 @@
         <v>50</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>11</v>
       </c>
@@ -1136,10 +1135,10 @@
         <v>46</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>11</v>
       </c>
@@ -1150,22 +1149,22 @@
         <v>142.02690000000001</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
@@ -1188,10 +1187,10 @@
         <v>34</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>20</v>
       </c>
@@ -1214,10 +1213,10 @@
         <v>35</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>20</v>
       </c>
@@ -1240,10 +1239,10 @@
         <v>45</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
@@ -1266,10 +1265,10 @@
         <v>36</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>24</v>
       </c>
@@ -1292,10 +1291,10 @@
         <v>37</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>18</v>
       </c>
@@ -1318,10 +1317,10 @@
         <v>38</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>18</v>
       </c>
@@ -1344,10 +1343,10 @@
         <v>39</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>18</v>
       </c>
@@ -1358,28 +1357,28 @@
         <v>186.01679999999999</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C32" s="3"/>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>4</v>
@@ -1388,24 +1387,24 @@
         <v>17.026548999999999</v>
       </c>
       <c r="D33" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="F33" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="E33" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="F33" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="G33" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B34" s="5" t="s">
         <v>4</v>
@@ -1414,24 +1413,24 @@
         <v>35.037114000000003</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H34" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="5" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>90</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>4</v>
@@ -1440,19 +1439,19 @@
         <v>18.010565</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>